<commit_message>
updating the CG coding, covariate coding, and adding descriptions for the CG data
</commit_message>
<xml_diff>
--- a/data-raw/BRFSS_SGM_CG_States_2015-2017.xlsx
+++ b/data-raw/BRFSS_SGM_CG_States_2015-2017.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcapistrant/Dropbox/BenAnalysis/BRFSS/brrfss/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B792504B-2DD4-934F-92CB-E92D93DCAE3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACCECF6-83A7-384A-84A6-092F0E9DA0C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="21600" windowHeight="38400" activeTab="2" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
   </bookViews>
   <sheets>
     <sheet name="CG_SGM_States" sheetId="2" r:id="rId1"/>
@@ -6653,8 +6653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34975563-31D7-A243-8C74-D0B76FAAE703}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B48" activeCellId="3" sqref="A33:XFD33 A35:XFD35 A40:XFD40 A48:XFD48"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6673,7 +6676,7 @@
     <col min="13" max="16384" width="5.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>84</v>
       </c>
@@ -6743,7 +6746,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="3">
-        <f>SUM(D2:J2)</f>
+        <f t="shared" ref="M2:M33" si="0">SUM(D2:J2)</f>
         <v>1</v>
       </c>
       <c r="N2" s="3">
@@ -6777,11 +6780,11 @@
         <v>76</v>
       </c>
       <c r="M3" s="3">
-        <f>SUM(D3:J3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N54" si="0">IF(OR(D3=1,G3=1,J3=1),1,0)</f>
+        <f t="shared" ref="N3:N54" si="1">IF(OR(D3=1,G3=1,J3=1),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -6811,11 +6814,11 @@
         <v>0</v>
       </c>
       <c r="M4" s="3">
-        <f>SUM(D4:J4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6845,11 +6848,11 @@
         <v>0</v>
       </c>
       <c r="M5" s="3">
-        <f>SUM(D5:J5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6880,11 +6883,11 @@
       </c>
       <c r="K6" s="4"/>
       <c r="M6" s="3">
-        <f>SUM(D6:J6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6915,11 +6918,11 @@
         <v>0</v>
       </c>
       <c r="M7" s="3">
-        <f>SUM(D7:J7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6951,11 +6954,11 @@
       </c>
       <c r="K8" s="4"/>
       <c r="M8" s="3">
-        <f>SUM(D8:J8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6982,11 +6985,11 @@
       </c>
       <c r="K9" s="4"/>
       <c r="M9" s="3">
-        <f>SUM(D9:J9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7016,11 +7019,11 @@
         <v>0</v>
       </c>
       <c r="M10" s="3">
-        <f>SUM(D10:J10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7051,11 +7054,11 @@
       </c>
       <c r="K11" s="4"/>
       <c r="M11" s="3">
-        <f>SUM(D11:J11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7087,11 +7090,11 @@
       </c>
       <c r="K12" s="4"/>
       <c r="M12" s="3">
-        <f>SUM(D12:J12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7108,11 +7111,11 @@
       <c r="H13" s="4"/>
       <c r="K13" s="4"/>
       <c r="M13" s="3">
-        <f>SUM(D13:J13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7149,11 +7152,11 @@
         <v>76</v>
       </c>
       <c r="M14" s="3">
-        <f>SUM(D14:J14)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7184,11 +7187,11 @@
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <f>SUM(D15:J15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7220,11 +7223,11 @@
       </c>
       <c r="K16" s="4"/>
       <c r="M16" s="3">
-        <f>SUM(D16:J16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7256,11 +7259,11 @@
       </c>
       <c r="K17" s="4"/>
       <c r="M17" s="3">
-        <f>SUM(D17:J17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7292,11 +7295,11 @@
       </c>
       <c r="K18" s="4"/>
       <c r="M18" s="3">
-        <f>SUM(D18:J18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7327,11 +7330,11 @@
         <v>77</v>
       </c>
       <c r="M19" s="3">
-        <f>SUM(D19:J19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7362,11 +7365,11 @@
         <v>0</v>
       </c>
       <c r="M20" s="3">
-        <f>SUM(D20:J20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7398,11 +7401,11 @@
       </c>
       <c r="K21" s="4"/>
       <c r="M21" s="3">
-        <f>SUM(D21:J21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7432,11 +7435,11 @@
         <v>0</v>
       </c>
       <c r="M22" s="3">
-        <f>SUM(D22:J22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7472,11 +7475,11 @@
         <v>151</v>
       </c>
       <c r="M23" s="3">
-        <f>SUM(D23:J23)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7502,11 +7505,11 @@
       </c>
       <c r="K24" s="4"/>
       <c r="M24" s="3">
-        <f>SUM(D24:J24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7536,11 +7539,11 @@
         <v>77</v>
       </c>
       <c r="M25" s="3">
-        <f>SUM(D25:J25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7572,11 +7575,11 @@
       </c>
       <c r="K26" s="4"/>
       <c r="M26" s="3">
-        <f>SUM(D26:J26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7608,11 +7611,11 @@
       </c>
       <c r="K27" s="4"/>
       <c r="M27" s="3">
-        <f>SUM(D27:J27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7643,11 +7646,11 @@
         <v>0</v>
       </c>
       <c r="M28" s="3">
-        <f>SUM(D28:J28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7678,11 +7681,11 @@
       </c>
       <c r="K29" s="4"/>
       <c r="M29" s="3">
-        <f>SUM(D29:J29)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7712,11 +7715,11 @@
         <v>0</v>
       </c>
       <c r="M30" s="3">
-        <f>SUM(D30:J30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7748,11 +7751,11 @@
       </c>
       <c r="K31" s="4"/>
       <c r="M31" s="3">
-        <f>SUM(D31:J31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7776,11 +7779,11 @@
         <v>0</v>
       </c>
       <c r="M32" s="3">
-        <f>SUM(D32:J32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7822,11 +7825,11 @@
         <v>77</v>
       </c>
       <c r="M33" s="3">
-        <f>SUM(D33:J33)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="N33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7856,11 +7859,11 @@
         <v>76</v>
       </c>
       <c r="M34" s="3">
-        <f>SUM(D34:J34)</f>
+        <f t="shared" ref="M34:M55" si="2">SUM(D34:J34)</f>
         <v>1</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7902,11 +7905,11 @@
         <v>147</v>
       </c>
       <c r="M35" s="3">
-        <f>SUM(D35:J35)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7930,11 +7933,11 @@
         <v>0</v>
       </c>
       <c r="M36" s="3">
-        <f>SUM(D36:J36)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7964,11 +7967,11 @@
         <v>0</v>
       </c>
       <c r="M37" s="3">
-        <f>SUM(D37:J37)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N37" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8000,11 +8003,11 @@
       </c>
       <c r="K38" s="4"/>
       <c r="M38" s="3">
-        <f>SUM(D38:J38)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8034,11 +8037,11 @@
         <v>147</v>
       </c>
       <c r="M39" s="3">
-        <f>SUM(D39:J39)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N39" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8080,11 +8083,11 @@
         <v>76</v>
       </c>
       <c r="M40" s="3">
-        <f>SUM(D40:J40)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N40" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8116,17 +8119,17 @@
       </c>
       <c r="K41" s="4"/>
       <c r="M41" s="3">
-        <f>SUM(D41:J41)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N41" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>126</v>
@@ -8150,11 +8153,11 @@
         <v>0</v>
       </c>
       <c r="M42" s="3">
-        <f>SUM(D42:J42)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N42" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8185,11 +8188,11 @@
         <v>76</v>
       </c>
       <c r="M43" s="3">
-        <f>SUM(D43:J43)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8219,11 +8222,11 @@
         <v>0</v>
       </c>
       <c r="M44" s="3">
-        <f>SUM(D44:J44)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N44" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8253,11 +8256,11 @@
         <v>0</v>
       </c>
       <c r="M45" s="3">
-        <f>SUM(D45:J45)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N45" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8293,11 +8296,11 @@
         <v>0</v>
       </c>
       <c r="M46" s="3">
-        <f>SUM(D46:J46)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="N46" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8329,11 +8332,11 @@
       </c>
       <c r="K47" s="4"/>
       <c r="M47" s="3">
-        <f>SUM(D47:J47)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N47" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8375,11 +8378,11 @@
         <v>147</v>
       </c>
       <c r="M48" s="3">
-        <f>SUM(D48:J48)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N48" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8406,11 +8409,11 @@
       </c>
       <c r="K49" s="4"/>
       <c r="M49" s="3">
-        <f>SUM(D49:J49)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N49" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8442,11 +8445,11 @@
       </c>
       <c r="K50" s="4"/>
       <c r="M50" s="3">
-        <f>SUM(D50:J50)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N50" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8472,11 +8475,11 @@
       </c>
       <c r="K51" s="4"/>
       <c r="M51" s="3">
-        <f>SUM(D51:J51)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N51" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8506,11 +8509,11 @@
         <v>0</v>
       </c>
       <c r="M52" s="3">
-        <f>SUM(D52:J52)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N52" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8542,11 +8545,11 @@
       </c>
       <c r="K53" s="4"/>
       <c r="M53" s="3">
-        <f>SUM(D53:J53)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N53" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8576,11 +8579,11 @@
         <v>0</v>
       </c>
       <c r="M54" s="3">
-        <f>SUM(D54:J54)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N54" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8598,7 +8601,7 @@
         <v>12</v>
       </c>
       <c r="M55" s="3">
-        <f>SUM(D55:J55)</f>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="N55" s="3">

</xml_diff>